<commit_message>
feat: parse excel by specific row and column
</commit_message>
<xml_diff>
--- a/sample/message.xlsx
+++ b/sample/message.xlsx
@@ -12,20 +12,41 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="45">
   <si>
     <t>Overview</t>
   </si>
   <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>World</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Alan</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
     <t>Output</t>
   </si>
   <si>
+    <t>Multiplicity</t>
+  </si>
+  <si>
     <t>Input</t>
   </si>
   <si>
     <t>world</t>
   </si>
   <si>
+    <t>[0..1]</t>
+  </si>
+  <si>
     <t xml:space="preserve">  asia</t>
   </si>
   <si>
@@ -99,6 +120,9 @@
   </si>
   <si>
     <t xml:space="preserve">        tokyo</t>
+  </si>
+  <si>
+    <t>[0..3]</t>
   </si>
   <si>
     <t xml:space="preserve">          shinjuku</t>
@@ -129,7 +153,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -143,6 +170,11 @@
       <b/>
     </font>
     <font/>
+    <font>
+      <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -152,23 +184,73 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border/>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -414,161 +496,272 @@
     <col customWidth="1" min="1" max="1" width="20.14"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="s">
+    <row r="2">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="D3" s="4"/>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="s">
+      <c r="C4" s="5">
+        <v>44159.0</v>
+      </c>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="6">
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="D6" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="s">
+      <c r="B7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="C7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="8"/>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="s">
+      <c r="B8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9">
+      <c r="B9" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="3" t="s">
+      <c r="C9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10">
+      <c r="B10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11">
+      <c r="B11" s="7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="3" t="s">
+      <c r="C11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="3" t="s">
+    <row r="12">
+      <c r="B12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="3" t="s">
+    <row r="13">
+      <c r="B13" s="7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="3" t="s">
+      <c r="C13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="1" t="s">
+    </row>
+    <row r="14">
+      <c r="B14" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="3" t="s">
+      <c r="C14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="1" t="s">
+    </row>
+    <row r="15">
+      <c r="B15" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="3" t="s">
+      <c r="C15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16">
+      <c r="B16" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="3" t="s">
+      <c r="C16" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="3" t="s">
+      <c r="B17" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="8"/>
+    </row>
+    <row r="18">
+      <c r="B18" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="3" t="s">
+      <c r="C18" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="9" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="s">
+      <c r="B19" s="7" t="s">
         <v>28</v>
       </c>
+      <c r="C19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="7" t="s">
         <v>30</v>
       </c>
+      <c r="C20" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="8"/>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="s">
+      <c r="B21" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="8"/>
+    </row>
+    <row r="22">
+      <c r="B22" s="7" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="s">
+      <c r="C22" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="1" t="s">
+    </row>
+    <row r="23">
+      <c r="B23" s="7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="3" t="s">
+      <c r="C23" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24">
+      <c r="B24" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C24" s="7" t="s">
         <v>36</v>
       </c>
+      <c r="D24" s="8"/>
+    </row>
+    <row r="25">
+      <c r="B25" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+  </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>